<commit_message>
Manutencao corretiva - correcao do cmd_incluir empresa
</commit_message>
<xml_diff>
--- a/sceweb/WebContent/WEB-INF/lib/roteiros_de_teste.xlsx
+++ b/sceweb/WebContent/WEB-INF/lib/roteiros_de_teste.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esa\git\scewebv2\sceweb\WebContent\WEB-INF\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esa\git\scewebv2x\sceweb\WebContent\WEB-INF\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>cadastro realizado com sucesso</t>
   </si>
@@ -108,6 +108,27 @@
   </si>
   <si>
     <t>excluirEmpresa</t>
+  </si>
+  <si>
+    <t>00656601000157</t>
+  </si>
+  <si>
+    <t>Kalunga</t>
+  </si>
+  <si>
+    <t>Kalunga loja</t>
+  </si>
+  <si>
+    <t>Rua Augusta</t>
+  </si>
+  <si>
+    <t>silva</t>
+  </si>
+  <si>
+    <t>faturamento</t>
+  </si>
+  <si>
+    <t>silva@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -474,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,21 +629,66 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="3">
+        <v>777788</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="3">
+        <v>666666</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M4" r:id="rId2" xr:uid="{26C5E87F-6E6B-4829-ACCB-DD77EF35FBE4}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>